<commit_message>
interação com input não clicável
</commit_message>
<xml_diff>
--- a/patrimonios.xlsx
+++ b/patrimonios.xlsx
@@ -17,6 +17,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t xml:space="preserve">teste</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -98,7 +106,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -115,23 +123,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
@@ -259,7 +269,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Página &amp;P</oddFooter>

</xml_diff>